<commit_message>
Release QRPH.mADX 3.0.0 as TI
</commit_message>
<xml_diff>
--- a/QRPH/mADX/StructureDefinition-mADX-Measure.xlsx
+++ b/QRPH/mADX/StructureDefinition-mADX-Measure.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4092" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4092" uniqueCount="587">
   <si>
     <t>Property</t>
   </si>
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>3.0.0-comment</t>
+    <t>3.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-03-24T16:19:35-05:00</t>
+    <t>2025-09-17T13:26:58-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -458,7 +458,7 @@
     <t>knowledgeCapability</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {cqf-knowledgeCapability}
+    <t xml:space="preserve">Extension {cqf-knowledgeCapability|5.2.0}
 </t>
   </si>
   <si>
@@ -474,7 +474,7 @@
     <t>artifactComment</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {cqf-artifactComment}
+    <t xml:space="preserve">Extension {cqf-artifactComment|5.2.0}
 </t>
   </si>
   <si>
@@ -490,7 +490,7 @@
     <t>versionAlgorithm</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {artifact-versionAlgorithm}
+    <t xml:space="preserve">Extension {artifact-versionAlgorithm|5.2.0}
 </t>
   </si>
   <si>
@@ -509,7 +509,7 @@
     <t>versionPolicy</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {artifact-versionPolicy}
+    <t xml:space="preserve">Extension {artifact-versionPolicy|5.2.0}
 </t>
   </si>
   <si>
@@ -1262,7 +1262,7 @@
 </t>
   </si>
   <si>
-    <t>There should be a related artifact for each dissagregation set defined under group[].stratifier[]</t>
+    <t>There should be a related artifact for each dissagregation set defined under group[].stratifier[].component[].code</t>
   </si>
   <si>
     <t>Related artifacts such as additional documentation, justification, or bibliographic references.</t>
@@ -1283,15 +1283,12 @@
     <t>Measure.relatedArtifact.type</t>
   </si>
   <si>
-    <t>documentation | justification | citation | predecessor | successor | derived-from | depends-on | composed-of</t>
+    <t>Should be set to 'depends-on' when referencing a disaggregating value set</t>
   </si>
   <si>
     <t>The type of relationship to the related artifact.</t>
   </si>
   <si>
-    <t>depends-on</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/ValueSet/related-artifact-type|4.0.1</t>
   </si>
   <si>
@@ -1301,7 +1298,7 @@
     <t>Measure.relatedArtifact.label</t>
   </si>
   <si>
-    <t>The label should match one of the values of group[].stratifier[].code for a disaggregation value set</t>
+    <t>The label should match one of the values of group[].stratifier[].component[].code for a disaggregation value set</t>
   </si>
   <si>
     <t>A short label that can be used to reference the citation from elsewhere in the containing artifact, such as a footnote index.</t>
@@ -1344,7 +1341,7 @@
 </t>
   </si>
   <si>
-    <t>The URL of a FHIR Valueset that defines the valid values reported in this disaggregation criterion as cross-referenced by relatedArtifact[].label</t>
+    <t>The URL of a FHIR value set that defines the valid values reported in this disaggregation criterion as cross-referenced by relatedArtifact[].label</t>
   </si>
   <si>
     <t>A url for the artifact that can be followed to access the actual content.</t>
@@ -1375,7 +1372,7 @@
     <t>Measure.relatedArtifact.resource</t>
   </si>
   <si>
-    <t xml:space="preserve">canonical(Resource)
+    <t xml:space="preserve">canonical(Resource|4.0.1)
 </t>
   </si>
   <si>
@@ -1635,7 +1632,7 @@
     <t>Measure.group.population.code</t>
   </si>
   <si>
-    <t>A required population code for a valid indicator. This code should be �numerator� if the reported indicator is a number (not a proportion). A proportion should have a numerator population and a denominator population</t>
+    <t>A required population code for a valid indicator.</t>
   </si>
   <si>
     <t>The type of population criteria.</t>
@@ -1693,7 +1690,7 @@
     <t>Measure.group.stratifier.code</t>
   </si>
   <si>
-    <t>There should be a code used to reference this disaggregating valueset. There must be a relatedArtifact for each disaggregation set which is a reference to a FHIR Valueset</t>
+    <t>Meaning of the stratifier</t>
   </si>
   <si>
     <t>Indicates a meaning for the stratifier. This can be as simple as a unique identifier, or it can establish meaning in a broader context by drawing from a terminology, allowing stratifiers to be correlated across measures.</t>
@@ -1720,7 +1717,7 @@
     <t>Measure.group.stratifier.component</t>
   </si>
   <si>
-    <t>Stratifier criteria component for the measure</t>
+    <t>There should be a 'component' for each set of disaggregators which is linked to a FHIR value set</t>
   </si>
   <si>
     <t>A component of the stratifier criteria for the measure report, specified as either the name of a valid CQL expression defined within a referenced library or a valid FHIR Resource Path.</t>
@@ -1741,7 +1738,7 @@
     <t>Measure.group.stratifier.component.code</t>
   </si>
   <si>
-    <t>Meaning of the stratifier component</t>
+    <t>There should be a code used to reference this disaggregating valueset. There must be a relatedArtifact for each disaggregation set which is a reference to a FHIR value set. The relatedArtifact.type should be set to 'depends-on'</t>
   </si>
   <si>
     <t>Indicates a meaning for the stratifier component. This can be as simple as a unique identifier, or it can establish meaning in a broader context by drawing from a terminology, allowing stratifiers to be correlated across measures.</t>
@@ -2170,17 +2167,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="59.6640625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="50.7578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="23.296875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="53.5078125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="45.51953125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="20.89453125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="34.8125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.29296875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.21484375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.55078125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.1171875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="10.75390625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="34.17578125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="35.5546875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -2189,26 +2186,26 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="8.84375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="134.4609375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="61.39453125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="44.47265625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="7.93359375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.08984375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="14.4296875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="15.31640625" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="14.62890625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="120.58984375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="55.0625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.10546875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="17.6953125" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="35.90625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="13.44140625" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="11.03515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="39.8828125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="8.51953125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="8.859375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="86.95703125" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="26.71875" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="32.84375" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="43.078125" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="77.984375" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="23.9609375" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="29.45703125" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="38.6328125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -8516,7 +8513,7 @@
         <v>80</v>
       </c>
       <c r="H56" t="s" s="2">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="I56" t="s" s="2">
         <v>79</v>
@@ -8540,7 +8537,7 @@
       </c>
       <c r="Q56" s="2"/>
       <c r="R56" t="s" s="2">
-        <v>411</v>
+        <v>79</v>
       </c>
       <c r="S56" t="s" s="2">
         <v>79</v>
@@ -8564,25 +8561,25 @@
         <v>410</v>
       </c>
       <c r="Z56" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="AA56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AB56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AC56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AD56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AE56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AF56" t="s" s="2">
         <v>412</v>
-      </c>
-      <c r="AA56" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AB56" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AC56" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AD56" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AE56" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AF56" t="s" s="2">
-        <v>413</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>80</v>
@@ -8611,10 +8608,10 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8622,13 +8619,13 @@
       </c>
       <c r="E57" s="2"/>
       <c r="F57" t="s" s="2">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G57" t="s" s="2">
         <v>80</v>
       </c>
       <c r="H57" t="s" s="2">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="I57" t="s" s="2">
         <v>79</v>
@@ -8640,10 +8637,10 @@
         <v>184</v>
       </c>
       <c r="L57" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="M57" t="s" s="2">
         <v>415</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>416</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
@@ -8694,7 +8691,7 @@
         <v>79</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>84</v>
@@ -8723,10 +8720,10 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8752,10 +8749,10 @@
         <v>184</v>
       </c>
       <c r="L58" t="s" s="2">
+        <v>418</v>
+      </c>
+      <c r="M58" t="s" s="2">
         <v>419</v>
-      </c>
-      <c r="M58" t="s" s="2">
-        <v>420</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
@@ -8806,7 +8803,7 @@
         <v>79</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>84</v>
@@ -8835,10 +8832,10 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8864,13 +8861,13 @@
         <v>326</v>
       </c>
       <c r="L59" t="s" s="2">
+        <v>422</v>
+      </c>
+      <c r="M59" t="s" s="2">
         <v>423</v>
       </c>
-      <c r="M59" t="s" s="2">
+      <c r="N59" t="s" s="2">
         <v>424</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>425</v>
       </c>
       <c r="O59" s="2"/>
       <c r="P59" t="s" s="2">
@@ -8920,7 +8917,7 @@
         <v>79</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>84</v>
@@ -8949,10 +8946,10 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8960,13 +8957,13 @@
       </c>
       <c r="E60" s="2"/>
       <c r="F60" t="s" s="2">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G60" t="s" s="2">
         <v>80</v>
       </c>
       <c r="H60" t="s" s="2">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="I60" t="s" s="2">
         <v>79</v>
@@ -8975,16 +8972,16 @@
         <v>89</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>427</v>
+      </c>
+      <c r="L60" t="s" s="2">
         <v>428</v>
       </c>
-      <c r="L60" t="s" s="2">
+      <c r="M60" t="s" s="2">
         <v>429</v>
       </c>
-      <c r="M60" t="s" s="2">
+      <c r="N60" t="s" s="2">
         <v>430</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>431</v>
       </c>
       <c r="O60" s="2"/>
       <c r="P60" t="s" s="2">
@@ -9034,7 +9031,7 @@
         <v>79</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>84</v>
@@ -9063,10 +9060,10 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -9089,13 +9086,13 @@
         <v>89</v>
       </c>
       <c r="K61" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="L61" t="s" s="2">
         <v>434</v>
       </c>
-      <c r="L61" t="s" s="2">
+      <c r="M61" t="s" s="2">
         <v>435</v>
-      </c>
-      <c r="M61" t="s" s="2">
-        <v>436</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -9146,7 +9143,7 @@
         <v>79</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>84</v>
@@ -9175,10 +9172,10 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -9201,16 +9198,16 @@
         <v>89</v>
       </c>
       <c r="K62" t="s" s="2">
+        <v>438</v>
+      </c>
+      <c r="L62" t="s" s="2">
         <v>439</v>
       </c>
-      <c r="L62" t="s" s="2">
+      <c r="M62" t="s" s="2">
         <v>440</v>
       </c>
-      <c r="M62" t="s" s="2">
+      <c r="N62" t="s" s="2">
         <v>441</v>
-      </c>
-      <c r="N62" t="s" s="2">
-        <v>442</v>
       </c>
       <c r="O62" s="2"/>
       <c r="P62" t="s" s="2">
@@ -9260,7 +9257,7 @@
         <v>79</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>84</v>
@@ -9289,10 +9286,10 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9315,13 +9312,13 @@
         <v>79</v>
       </c>
       <c r="K63" t="s" s="2">
+        <v>444</v>
+      </c>
+      <c r="L63" t="s" s="2">
         <v>445</v>
       </c>
-      <c r="L63" t="s" s="2">
+      <c r="M63" t="s" s="2">
         <v>446</v>
-      </c>
-      <c r="M63" t="s" s="2">
-        <v>447</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
@@ -9372,7 +9369,7 @@
         <v>79</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>84</v>
@@ -9401,10 +9398,10 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
@@ -9430,14 +9427,14 @@
         <v>326</v>
       </c>
       <c r="L64" t="s" s="2">
+        <v>448</v>
+      </c>
+      <c r="M64" t="s" s="2">
         <v>449</v>
-      </c>
-      <c r="M64" t="s" s="2">
-        <v>450</v>
       </c>
       <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P64" t="s" s="2">
         <v>79</v>
@@ -9486,7 +9483,7 @@
         <v>79</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>84</v>
@@ -9515,10 +9512,10 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9544,10 +9541,10 @@
         <v>221</v>
       </c>
       <c r="L65" t="s" s="2">
+        <v>452</v>
+      </c>
+      <c r="M65" t="s" s="2">
         <v>453</v>
-      </c>
-      <c r="M65" t="s" s="2">
-        <v>454</v>
       </c>
       <c r="N65" s="2"/>
       <c r="O65" s="2"/>
@@ -9577,11 +9574,11 @@
         <v>226</v>
       </c>
       <c r="Y65" t="s" s="2">
+        <v>454</v>
+      </c>
+      <c r="Z65" t="s" s="2">
         <v>455</v>
       </c>
-      <c r="Z65" t="s" s="2">
-        <v>456</v>
-      </c>
       <c r="AA65" t="s" s="2">
         <v>79</v>
       </c>
@@ -9598,7 +9595,7 @@
         <v>79</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="AG65" t="s" s="2">
         <v>84</v>
@@ -9627,10 +9624,10 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -9656,10 +9653,10 @@
         <v>221</v>
       </c>
       <c r="L66" t="s" s="2">
+        <v>457</v>
+      </c>
+      <c r="M66" t="s" s="2">
         <v>458</v>
-      </c>
-      <c r="M66" t="s" s="2">
-        <v>459</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" s="2"/>
@@ -9689,11 +9686,11 @@
         <v>226</v>
       </c>
       <c r="Y66" t="s" s="2">
+        <v>459</v>
+      </c>
+      <c r="Z66" t="s" s="2">
         <v>460</v>
       </c>
-      <c r="Z66" t="s" s="2">
-        <v>461</v>
-      </c>
       <c r="AA66" t="s" s="2">
         <v>79</v>
       </c>
@@ -9710,7 +9707,7 @@
         <v>79</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>84</v>
@@ -9739,10 +9736,10 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
@@ -9768,10 +9765,10 @@
         <v>221</v>
       </c>
       <c r="L67" t="s" s="2">
+        <v>462</v>
+      </c>
+      <c r="M67" t="s" s="2">
         <v>463</v>
-      </c>
-      <c r="M67" t="s" s="2">
-        <v>464</v>
       </c>
       <c r="N67" s="2"/>
       <c r="O67" s="2"/>
@@ -9801,11 +9798,11 @@
         <v>226</v>
       </c>
       <c r="Y67" t="s" s="2">
+        <v>464</v>
+      </c>
+      <c r="Z67" t="s" s="2">
         <v>465</v>
       </c>
-      <c r="Z67" t="s" s="2">
-        <v>466</v>
-      </c>
       <c r="AA67" t="s" s="2">
         <v>79</v>
       </c>
@@ -9822,7 +9819,7 @@
         <v>79</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>84</v>
@@ -9851,10 +9848,10 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" t="s" s="2">
@@ -9880,13 +9877,13 @@
         <v>184</v>
       </c>
       <c r="L68" t="s" s="2">
+        <v>467</v>
+      </c>
+      <c r="M68" t="s" s="2">
         <v>468</v>
       </c>
-      <c r="M68" t="s" s="2">
+      <c r="N68" t="s" s="2">
         <v>469</v>
-      </c>
-      <c r="N68" t="s" s="2">
-        <v>470</v>
       </c>
       <c r="O68" s="2"/>
       <c r="P68" t="s" s="2">
@@ -9936,7 +9933,7 @@
         <v>79</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AG68" t="s" s="2">
         <v>84</v>
@@ -9965,10 +9962,10 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
@@ -9994,13 +9991,13 @@
         <v>184</v>
       </c>
       <c r="L69" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="M69" t="s" s="2">
         <v>472</v>
       </c>
-      <c r="M69" t="s" s="2">
+      <c r="N69" t="s" s="2">
         <v>473</v>
-      </c>
-      <c r="N69" t="s" s="2">
-        <v>474</v>
       </c>
       <c r="O69" s="2"/>
       <c r="P69" t="s" s="2">
@@ -10050,7 +10047,7 @@
         <v>79</v>
       </c>
       <c r="AF69" t="s" s="2">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="AG69" t="s" s="2">
         <v>84</v>
@@ -10079,10 +10076,10 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
@@ -10108,14 +10105,14 @@
         <v>326</v>
       </c>
       <c r="L70" t="s" s="2">
+        <v>475</v>
+      </c>
+      <c r="M70" t="s" s="2">
         <v>476</v>
-      </c>
-      <c r="M70" t="s" s="2">
-        <v>477</v>
       </c>
       <c r="N70" s="2"/>
       <c r="O70" t="s" s="2">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="P70" t="s" s="2">
         <v>79</v>
@@ -10164,7 +10161,7 @@
         <v>79</v>
       </c>
       <c r="AF70" t="s" s="2">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="AG70" t="s" s="2">
         <v>84</v>
@@ -10193,10 +10190,10 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
@@ -10222,10 +10219,10 @@
         <v>326</v>
       </c>
       <c r="L71" t="s" s="2">
+        <v>479</v>
+      </c>
+      <c r="M71" t="s" s="2">
         <v>480</v>
-      </c>
-      <c r="M71" t="s" s="2">
-        <v>481</v>
       </c>
       <c r="N71" s="2"/>
       <c r="O71" s="2"/>
@@ -10276,7 +10273,7 @@
         <v>79</v>
       </c>
       <c r="AF71" t="s" s="2">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AG71" t="s" s="2">
         <v>84</v>
@@ -10305,10 +10302,10 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -10316,13 +10313,13 @@
       </c>
       <c r="E72" s="2"/>
       <c r="F72" t="s" s="2">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G72" t="s" s="2">
         <v>80</v>
       </c>
       <c r="H72" t="s" s="2">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="I72" t="s" s="2">
         <v>79</v>
@@ -10334,14 +10331,14 @@
         <v>221</v>
       </c>
       <c r="L72" t="s" s="2">
+        <v>482</v>
+      </c>
+      <c r="M72" t="s" s="2">
         <v>483</v>
-      </c>
-      <c r="M72" t="s" s="2">
-        <v>484</v>
       </c>
       <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P72" t="s" s="2">
         <v>79</v>
@@ -10369,11 +10366,11 @@
         <v>208</v>
       </c>
       <c r="Y72" t="s" s="2">
+        <v>485</v>
+      </c>
+      <c r="Z72" t="s" s="2">
         <v>486</v>
       </c>
-      <c r="Z72" t="s" s="2">
-        <v>487</v>
-      </c>
       <c r="AA72" t="s" s="2">
         <v>79</v>
       </c>
@@ -10390,7 +10387,7 @@
         <v>79</v>
       </c>
       <c r="AF72" t="s" s="2">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AG72" t="s" s="2">
         <v>84</v>
@@ -10419,10 +10416,10 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -10448,14 +10445,14 @@
         <v>326</v>
       </c>
       <c r="L73" t="s" s="2">
+        <v>488</v>
+      </c>
+      <c r="M73" t="s" s="2">
         <v>489</v>
-      </c>
-      <c r="M73" t="s" s="2">
-        <v>490</v>
       </c>
       <c r="N73" s="2"/>
       <c r="O73" t="s" s="2">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="P73" t="s" s="2">
         <v>79</v>
@@ -10504,7 +10501,7 @@
         <v>79</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="AG73" t="s" s="2">
         <v>84</v>
@@ -10533,10 +10530,10 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
@@ -10562,14 +10559,14 @@
         <v>326</v>
       </c>
       <c r="L74" t="s" s="2">
+        <v>492</v>
+      </c>
+      <c r="M74" t="s" s="2">
         <v>493</v>
-      </c>
-      <c r="M74" t="s" s="2">
-        <v>494</v>
       </c>
       <c r="N74" s="2"/>
       <c r="O74" t="s" s="2">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="P74" t="s" s="2">
         <v>79</v>
@@ -10618,7 +10615,7 @@
         <v>79</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>84</v>
@@ -10647,10 +10644,10 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
@@ -10673,13 +10670,13 @@
         <v>79</v>
       </c>
       <c r="K75" t="s" s="2">
+        <v>496</v>
+      </c>
+      <c r="L75" t="s" s="2">
         <v>497</v>
       </c>
-      <c r="L75" t="s" s="2">
+      <c r="M75" t="s" s="2">
         <v>498</v>
-      </c>
-      <c r="M75" t="s" s="2">
-        <v>499</v>
       </c>
       <c r="N75" s="2"/>
       <c r="O75" s="2"/>
@@ -10730,7 +10727,7 @@
         <v>79</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="AG75" t="s" s="2">
         <v>84</v>
@@ -10759,10 +10756,10 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" t="s" s="2">
@@ -10871,10 +10868,10 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
@@ -10985,14 +10982,14 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" t="s" s="2">
@@ -11014,10 +11011,10 @@
         <v>133</v>
       </c>
       <c r="L78" t="s" s="2">
+        <v>503</v>
+      </c>
+      <c r="M78" t="s" s="2">
         <v>504</v>
-      </c>
-      <c r="M78" t="s" s="2">
-        <v>505</v>
       </c>
       <c r="N78" t="s" s="2">
         <v>165</v>
@@ -11072,7 +11069,7 @@
         <v>79</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>84</v>
@@ -11101,10 +11098,10 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B79" t="s" s="2">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" t="s" s="2">
@@ -11130,10 +11127,10 @@
         <v>221</v>
       </c>
       <c r="L79" t="s" s="2">
+        <v>507</v>
+      </c>
+      <c r="M79" t="s" s="2">
         <v>508</v>
-      </c>
-      <c r="M79" t="s" s="2">
-        <v>509</v>
       </c>
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
@@ -11184,7 +11181,7 @@
         <v>79</v>
       </c>
       <c r="AF79" t="s" s="2">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="AG79" t="s" s="2">
         <v>84</v>
@@ -11213,10 +11210,10 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" t="s" s="2">
@@ -11325,10 +11322,10 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s" s="2">
@@ -11439,10 +11436,10 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B82" t="s" s="2">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" t="s" s="2">
@@ -11555,10 +11552,10 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B83" t="s" s="2">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" t="s" s="2">
@@ -11671,10 +11668,10 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B84" t="s" s="2">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" t="s" s="2">
@@ -11700,10 +11697,10 @@
         <v>184</v>
       </c>
       <c r="L84" t="s" s="2">
+        <v>514</v>
+      </c>
+      <c r="M84" t="s" s="2">
         <v>515</v>
-      </c>
-      <c r="M84" t="s" s="2">
-        <v>516</v>
       </c>
       <c r="N84" s="2"/>
       <c r="O84" s="2"/>
@@ -11754,7 +11751,7 @@
         <v>79</v>
       </c>
       <c r="AF84" t="s" s="2">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="AG84" t="s" s="2">
         <v>84</v>
@@ -11783,10 +11780,10 @@
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" t="s" s="2">
@@ -11809,13 +11806,13 @@
         <v>79</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="L85" t="s" s="2">
+        <v>517</v>
+      </c>
+      <c r="M85" t="s" s="2">
         <v>518</v>
-      </c>
-      <c r="M85" t="s" s="2">
-        <v>519</v>
       </c>
       <c r="N85" s="2"/>
       <c r="O85" s="2"/>
@@ -11866,7 +11863,7 @@
         <v>79</v>
       </c>
       <c r="AF85" t="s" s="2">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="AG85" t="s" s="2">
         <v>84</v>
@@ -11895,10 +11892,10 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B86" t="s" s="2">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" t="s" s="2">
@@ -12007,10 +12004,10 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B87" t="s" s="2">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" t="s" s="2">
@@ -12121,14 +12118,14 @@
     </row>
     <row r="88" hidden="true">
       <c r="A88" t="s" s="2">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B88" t="s" s="2">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" t="s" s="2">
@@ -12150,10 +12147,10 @@
         <v>133</v>
       </c>
       <c r="L88" t="s" s="2">
+        <v>503</v>
+      </c>
+      <c r="M88" t="s" s="2">
         <v>504</v>
-      </c>
-      <c r="M88" t="s" s="2">
-        <v>505</v>
       </c>
       <c r="N88" t="s" s="2">
         <v>165</v>
@@ -12208,7 +12205,7 @@
         <v>79</v>
       </c>
       <c r="AF88" t="s" s="2">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="AG88" t="s" s="2">
         <v>84</v>
@@ -12237,10 +12234,10 @@
     </row>
     <row r="89" hidden="true">
       <c r="A89" t="s" s="2">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B89" t="s" s="2">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" t="s" s="2">
@@ -12266,10 +12263,10 @@
         <v>221</v>
       </c>
       <c r="L89" t="s" s="2">
+        <v>523</v>
+      </c>
+      <c r="M89" t="s" s="2">
         <v>524</v>
-      </c>
-      <c r="M89" t="s" s="2">
-        <v>525</v>
       </c>
       <c r="N89" s="2"/>
       <c r="O89" s="2"/>
@@ -12299,11 +12296,11 @@
         <v>226</v>
       </c>
       <c r="Y89" t="s" s="2">
+        <v>525</v>
+      </c>
+      <c r="Z89" t="s" s="2">
         <v>526</v>
       </c>
-      <c r="Z89" t="s" s="2">
-        <v>527</v>
-      </c>
       <c r="AA89" t="s" s="2">
         <v>79</v>
       </c>
@@ -12320,7 +12317,7 @@
         <v>79</v>
       </c>
       <c r="AF89" t="s" s="2">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="AG89" t="s" s="2">
         <v>84</v>
@@ -12349,10 +12346,10 @@
     </row>
     <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B90" t="s" s="2">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" t="s" s="2">
@@ -12378,10 +12375,10 @@
         <v>184</v>
       </c>
       <c r="L90" t="s" s="2">
+        <v>528</v>
+      </c>
+      <c r="M90" t="s" s="2">
         <v>529</v>
-      </c>
-      <c r="M90" t="s" s="2">
-        <v>530</v>
       </c>
       <c r="N90" s="2"/>
       <c r="O90" s="2"/>
@@ -12432,7 +12429,7 @@
         <v>79</v>
       </c>
       <c r="AF90" t="s" s="2">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="AG90" t="s" s="2">
         <v>84</v>
@@ -12461,10 +12458,10 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B91" t="s" s="2">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" t="s" s="2">
@@ -12487,16 +12484,16 @@
         <v>79</v>
       </c>
       <c r="K91" t="s" s="2">
+        <v>531</v>
+      </c>
+      <c r="L91" t="s" s="2">
         <v>532</v>
       </c>
-      <c r="L91" t="s" s="2">
+      <c r="M91" t="s" s="2">
         <v>533</v>
       </c>
-      <c r="M91" t="s" s="2">
+      <c r="N91" t="s" s="2">
         <v>534</v>
-      </c>
-      <c r="N91" t="s" s="2">
-        <v>535</v>
       </c>
       <c r="O91" s="2"/>
       <c r="P91" t="s" s="2">
@@ -12546,7 +12543,7 @@
         <v>79</v>
       </c>
       <c r="AF91" t="s" s="2">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="AG91" t="s" s="2">
         <v>80</v>
@@ -12575,10 +12572,10 @@
     </row>
     <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B92" t="s" s="2">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" t="s" s="2">
@@ -12601,13 +12598,13 @@
         <v>79</v>
       </c>
       <c r="K92" t="s" s="2">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="L92" t="s" s="2">
+        <v>536</v>
+      </c>
+      <c r="M92" t="s" s="2">
         <v>537</v>
-      </c>
-      <c r="M92" t="s" s="2">
-        <v>538</v>
       </c>
       <c r="N92" s="2"/>
       <c r="O92" s="2"/>
@@ -12658,7 +12655,7 @@
         <v>79</v>
       </c>
       <c r="AF92" t="s" s="2">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="AG92" t="s" s="2">
         <v>84</v>
@@ -12687,10 +12684,10 @@
     </row>
     <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B93" t="s" s="2">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" t="s" s="2">
@@ -12799,10 +12796,10 @@
     </row>
     <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B94" t="s" s="2">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" t="s" s="2">
@@ -12913,14 +12910,14 @@
     </row>
     <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B95" t="s" s="2">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95" t="s" s="2">
@@ -12942,10 +12939,10 @@
         <v>133</v>
       </c>
       <c r="L95" t="s" s="2">
+        <v>503</v>
+      </c>
+      <c r="M95" t="s" s="2">
         <v>504</v>
-      </c>
-      <c r="M95" t="s" s="2">
-        <v>505</v>
       </c>
       <c r="N95" t="s" s="2">
         <v>165</v>
@@ -13000,7 +12997,7 @@
         <v>79</v>
       </c>
       <c r="AF95" t="s" s="2">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="AG95" t="s" s="2">
         <v>84</v>
@@ -13029,10 +13026,10 @@
     </row>
     <row r="96" hidden="true">
       <c r="A96" t="s" s="2">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B96" t="s" s="2">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" t="s" s="2">
@@ -13046,7 +13043,7 @@
         <v>80</v>
       </c>
       <c r="H96" t="s" s="2">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="I96" t="s" s="2">
         <v>79</v>
@@ -13058,10 +13055,10 @@
         <v>221</v>
       </c>
       <c r="L96" t="s" s="2">
+        <v>542</v>
+      </c>
+      <c r="M96" t="s" s="2">
         <v>543</v>
-      </c>
-      <c r="M96" t="s" s="2">
-        <v>544</v>
       </c>
       <c r="N96" s="2"/>
       <c r="O96" s="2"/>
@@ -13112,7 +13109,7 @@
         <v>79</v>
       </c>
       <c r="AF96" t="s" s="2">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AG96" t="s" s="2">
         <v>84</v>
@@ -13141,10 +13138,10 @@
     </row>
     <row r="97" hidden="true">
       <c r="A97" t="s" s="2">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B97" t="s" s="2">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" t="s" s="2">
@@ -13170,10 +13167,10 @@
         <v>184</v>
       </c>
       <c r="L97" t="s" s="2">
+        <v>545</v>
+      </c>
+      <c r="M97" t="s" s="2">
         <v>546</v>
-      </c>
-      <c r="M97" t="s" s="2">
-        <v>547</v>
       </c>
       <c r="N97" s="2"/>
       <c r="O97" s="2"/>
@@ -13224,7 +13221,7 @@
         <v>79</v>
       </c>
       <c r="AF97" t="s" s="2">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="AG97" t="s" s="2">
         <v>84</v>
@@ -13253,10 +13250,10 @@
     </row>
     <row r="98" hidden="true">
       <c r="A98" t="s" s="2">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B98" t="s" s="2">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" t="s" s="2">
@@ -13279,13 +13276,13 @@
         <v>79</v>
       </c>
       <c r="K98" t="s" s="2">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L98" t="s" s="2">
+        <v>548</v>
+      </c>
+      <c r="M98" t="s" s="2">
         <v>549</v>
-      </c>
-      <c r="M98" t="s" s="2">
-        <v>550</v>
       </c>
       <c r="N98" s="2"/>
       <c r="O98" s="2"/>
@@ -13336,7 +13333,7 @@
         <v>79</v>
       </c>
       <c r="AF98" t="s" s="2">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AG98" t="s" s="2">
         <v>84</v>
@@ -13365,10 +13362,10 @@
     </row>
     <row r="99" hidden="true">
       <c r="A99" t="s" s="2">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B99" t="s" s="2">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" t="s" s="2">
@@ -13382,7 +13379,7 @@
         <v>85</v>
       </c>
       <c r="H99" t="s" s="2">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="I99" t="s" s="2">
         <v>79</v>
@@ -13391,16 +13388,16 @@
         <v>79</v>
       </c>
       <c r="K99" t="s" s="2">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="L99" t="s" s="2">
+        <v>551</v>
+      </c>
+      <c r="M99" t="s" s="2">
         <v>552</v>
       </c>
-      <c r="M99" t="s" s="2">
+      <c r="N99" t="s" s="2">
         <v>553</v>
-      </c>
-      <c r="N99" t="s" s="2">
-        <v>554</v>
       </c>
       <c r="O99" s="2"/>
       <c r="P99" t="s" s="2">
@@ -13450,7 +13447,7 @@
         <v>79</v>
       </c>
       <c r="AF99" t="s" s="2">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="AG99" t="s" s="2">
         <v>84</v>
@@ -13479,10 +13476,10 @@
     </row>
     <row r="100" hidden="true">
       <c r="A100" t="s" s="2">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B100" t="s" s="2">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" t="s" s="2">
@@ -13591,10 +13588,10 @@
     </row>
     <row r="101" hidden="true">
       <c r="A101" t="s" s="2">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B101" t="s" s="2">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" t="s" s="2">
@@ -13705,14 +13702,14 @@
     </row>
     <row r="102" hidden="true">
       <c r="A102" t="s" s="2">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B102" t="s" s="2">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102" t="s" s="2">
@@ -13734,10 +13731,10 @@
         <v>133</v>
       </c>
       <c r="L102" t="s" s="2">
+        <v>503</v>
+      </c>
+      <c r="M102" t="s" s="2">
         <v>504</v>
-      </c>
-      <c r="M102" t="s" s="2">
-        <v>505</v>
       </c>
       <c r="N102" t="s" s="2">
         <v>165</v>
@@ -13792,7 +13789,7 @@
         <v>79</v>
       </c>
       <c r="AF102" t="s" s="2">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="AG102" t="s" s="2">
         <v>84</v>
@@ -13821,10 +13818,10 @@
     </row>
     <row r="103" hidden="true">
       <c r="A103" t="s" s="2">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B103" t="s" s="2">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" t="s" s="2">
@@ -13838,7 +13835,7 @@
         <v>80</v>
       </c>
       <c r="H103" t="s" s="2">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="I103" t="s" s="2">
         <v>79</v>
@@ -13850,10 +13847,10 @@
         <v>221</v>
       </c>
       <c r="L103" t="s" s="2">
+        <v>558</v>
+      </c>
+      <c r="M103" t="s" s="2">
         <v>559</v>
-      </c>
-      <c r="M103" t="s" s="2">
-        <v>560</v>
       </c>
       <c r="N103" s="2"/>
       <c r="O103" s="2"/>
@@ -13904,7 +13901,7 @@
         <v>79</v>
       </c>
       <c r="AF103" t="s" s="2">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="AG103" t="s" s="2">
         <v>84</v>
@@ -13933,10 +13930,10 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B104" t="s" s="2">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" t="s" s="2">
@@ -13962,10 +13959,10 @@
         <v>184</v>
       </c>
       <c r="L104" t="s" s="2">
+        <v>561</v>
+      </c>
+      <c r="M104" t="s" s="2">
         <v>562</v>
-      </c>
-      <c r="M104" t="s" s="2">
-        <v>563</v>
       </c>
       <c r="N104" s="2"/>
       <c r="O104" s="2"/>
@@ -14016,7 +14013,7 @@
         <v>79</v>
       </c>
       <c r="AF104" t="s" s="2">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="AG104" t="s" s="2">
         <v>84</v>
@@ -14045,10 +14042,10 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B105" t="s" s="2">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" t="s" s="2">
@@ -14071,13 +14068,13 @@
         <v>79</v>
       </c>
       <c r="K105" t="s" s="2">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L105" t="s" s="2">
+        <v>564</v>
+      </c>
+      <c r="M105" t="s" s="2">
         <v>565</v>
-      </c>
-      <c r="M105" t="s" s="2">
-        <v>566</v>
       </c>
       <c r="N105" s="2"/>
       <c r="O105" s="2"/>
@@ -14128,7 +14125,7 @@
         <v>79</v>
       </c>
       <c r="AF105" t="s" s="2">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="AG105" t="s" s="2">
         <v>80</v>
@@ -14157,10 +14154,10 @@
     </row>
     <row r="106" hidden="true">
       <c r="A106" t="s" s="2">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B106" t="s" s="2">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C106" s="2"/>
       <c r="D106" t="s" s="2">
@@ -14183,16 +14180,16 @@
         <v>79</v>
       </c>
       <c r="K106" t="s" s="2">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="L106" t="s" s="2">
+        <v>567</v>
+      </c>
+      <c r="M106" t="s" s="2">
         <v>568</v>
       </c>
-      <c r="M106" t="s" s="2">
+      <c r="N106" t="s" s="2">
         <v>569</v>
-      </c>
-      <c r="N106" t="s" s="2">
-        <v>570</v>
       </c>
       <c r="O106" s="2"/>
       <c r="P106" t="s" s="2">
@@ -14242,7 +14239,7 @@
         <v>79</v>
       </c>
       <c r="AF106" t="s" s="2">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="AG106" t="s" s="2">
         <v>84</v>
@@ -14271,10 +14268,10 @@
     </row>
     <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B107" t="s" s="2">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C107" s="2"/>
       <c r="D107" t="s" s="2">
@@ -14383,10 +14380,10 @@
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B108" t="s" s="2">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" t="s" s="2">
@@ -14497,14 +14494,14 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B109" t="s" s="2">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E109" s="2"/>
       <c r="F109" t="s" s="2">
@@ -14526,10 +14523,10 @@
         <v>133</v>
       </c>
       <c r="L109" t="s" s="2">
+        <v>503</v>
+      </c>
+      <c r="M109" t="s" s="2">
         <v>504</v>
-      </c>
-      <c r="M109" t="s" s="2">
-        <v>505</v>
       </c>
       <c r="N109" t="s" s="2">
         <v>165</v>
@@ -14584,7 +14581,7 @@
         <v>79</v>
       </c>
       <c r="AF109" t="s" s="2">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="AG109" t="s" s="2">
         <v>84</v>
@@ -14613,10 +14610,10 @@
     </row>
     <row r="110" hidden="true">
       <c r="A110" t="s" s="2">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B110" t="s" s="2">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C110" s="2"/>
       <c r="D110" t="s" s="2">
@@ -14642,10 +14639,10 @@
         <v>221</v>
       </c>
       <c r="L110" t="s" s="2">
+        <v>574</v>
+      </c>
+      <c r="M110" t="s" s="2">
         <v>575</v>
-      </c>
-      <c r="M110" t="s" s="2">
-        <v>576</v>
       </c>
       <c r="N110" s="2"/>
       <c r="O110" s="2"/>
@@ -14696,7 +14693,7 @@
         <v>79</v>
       </c>
       <c r="AF110" t="s" s="2">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="AG110" t="s" s="2">
         <v>84</v>
@@ -14725,10 +14722,10 @@
     </row>
     <row r="111" hidden="true">
       <c r="A111" t="s" s="2">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B111" t="s" s="2">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" t="s" s="2">
@@ -14754,10 +14751,10 @@
         <v>221</v>
       </c>
       <c r="L111" t="s" s="2">
+        <v>577</v>
+      </c>
+      <c r="M111" t="s" s="2">
         <v>578</v>
-      </c>
-      <c r="M111" t="s" s="2">
-        <v>579</v>
       </c>
       <c r="N111" s="2"/>
       <c r="O111" s="2"/>
@@ -14787,11 +14784,11 @@
         <v>226</v>
       </c>
       <c r="Y111" t="s" s="2">
+        <v>579</v>
+      </c>
+      <c r="Z111" t="s" s="2">
         <v>580</v>
       </c>
-      <c r="Z111" t="s" s="2">
-        <v>581</v>
-      </c>
       <c r="AA111" t="s" s="2">
         <v>79</v>
       </c>
@@ -14808,7 +14805,7 @@
         <v>79</v>
       </c>
       <c r="AF111" t="s" s="2">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="AG111" t="s" s="2">
         <v>84</v>
@@ -14837,10 +14834,10 @@
     </row>
     <row r="112" hidden="true">
       <c r="A112" t="s" s="2">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B112" t="s" s="2">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" t="s" s="2">
@@ -14866,10 +14863,10 @@
         <v>184</v>
       </c>
       <c r="L112" t="s" s="2">
+        <v>582</v>
+      </c>
+      <c r="M112" t="s" s="2">
         <v>583</v>
-      </c>
-      <c r="M112" t="s" s="2">
-        <v>584</v>
       </c>
       <c r="N112" s="2"/>
       <c r="O112" s="2"/>
@@ -14920,7 +14917,7 @@
         <v>79</v>
       </c>
       <c r="AF112" t="s" s="2">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AG112" t="s" s="2">
         <v>84</v>
@@ -14949,10 +14946,10 @@
     </row>
     <row r="113" hidden="true">
       <c r="A113" t="s" s="2">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B113" t="s" s="2">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" t="s" s="2">
@@ -14975,13 +14972,13 @@
         <v>79</v>
       </c>
       <c r="K113" t="s" s="2">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="L113" t="s" s="2">
+        <v>585</v>
+      </c>
+      <c r="M113" t="s" s="2">
         <v>586</v>
-      </c>
-      <c r="M113" t="s" s="2">
-        <v>587</v>
       </c>
       <c r="N113" s="2"/>
       <c r="O113" s="2"/>
@@ -15032,7 +15029,7 @@
         <v>79</v>
       </c>
       <c r="AF113" t="s" s="2">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="AG113" t="s" s="2">
         <v>80</v>

</xml_diff>